<commit_message>
updated customflow objects ans service classes
</commit_message>
<xml_diff>
--- a/customflows/src/main/resources/TestData/CustomFlowSettings.xlsx
+++ b/customflows/src/main/resources/TestData/CustomFlowSettings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Automation\Automation_Project\customflows\src\main\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EFBDEE1-2356-4B34-B4A5-BA96957D16BE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6FFC341-09B5-40EC-B46B-96343E1636BF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="908" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="908" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CFForm" sheetId="5" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="102">
   <si>
     <t>Description</t>
   </si>
@@ -243,9 +243,6 @@
     <t>Initiator</t>
   </si>
   <si>
-    <t>CF Approval Flow 2 stage Auto</t>
-  </si>
-  <si>
     <t>form:</t>
   </si>
   <si>
@@ -318,9 +315,6 @@
     <t>3,269</t>
   </si>
   <si>
-    <t>1,7</t>
-  </si>
-  <si>
     <t>CF Approval Flow  3 stage Auto</t>
   </si>
   <si>
@@ -340,6 +334,12 @@
   </si>
   <si>
     <t>VisibilityRoles</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Subject</t>
   </si>
 </sst>
 </file>
@@ -698,10 +698,10 @@
         <v>21</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -715,7 +715,7 @@
         <v>62</v>
       </c>
       <c r="D2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E2" t="s">
         <v>40</v>
@@ -723,7 +723,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B3" t="s">
         <v>40</v>
@@ -732,7 +732,7 @@
         <v>64</v>
       </c>
       <c r="D3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E3" t="s">
         <v>40</v>
@@ -876,7 +876,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B5" t="s">
         <v>56</v>
@@ -1072,10 +1072,10 @@
         <v>25</v>
       </c>
       <c r="F2" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>90</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>91</v>
       </c>
       <c r="H2" t="s">
         <v>25</v>
@@ -1089,19 +1089,19 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="6" t="s">
         <v>89</v>
-      </c>
-      <c r="C3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>90</v>
       </c>
       <c r="H3" t="s">
         <v>25</v>
@@ -1118,10 +1118,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D99226C-5D02-4BBA-A400-810643F45BAE}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1140,7 +1140,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B2" t="s">
         <v>62</v>
@@ -1148,17 +1148,9 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B4" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1170,24 +1162,25 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64379857-4A16-4890-9E2A-322439F6ECD4}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.5703125" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" customWidth="1"/>
+    <col min="8" max="8" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
@@ -1195,150 +1188,170 @@
         <v>29</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>101</v>
-      </c>
       <c r="F1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>64</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1"/>
+      <c r="E2" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="F2" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B3" t="s">
         <v>91</v>
       </c>
-      <c r="B3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="B4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E4" t="s">
         <v>68</v>
       </c>
-      <c r="E3" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="F3" s="2" t="s">
+      <c r="F4" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="B4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D4" t="s">
-        <v>68</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
       <c r="B5" t="s">
         <v>41</v>
       </c>
-      <c r="D5" t="s">
+      <c r="C5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" t="s">
         <v>68</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>2</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="H5" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B6" t="s">
         <v>55</v>
       </c>
       <c r="C6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" t="s">
         <v>61</v>
       </c>
-      <c r="E6" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F7" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="C7" t="s">
-        <v>60</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
       <c r="B8" t="s">
         <v>57</v>
       </c>
-      <c r="E8">
+      <c r="C8" t="s">
+        <v>57</v>
+      </c>
+      <c r="F8">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3</v>
       </c>
@@ -1346,22 +1359,36 @@
         <v>58</v>
       </c>
       <c r="C9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" t="s">
         <v>62</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>3</v>
       </c>
       <c r="B10" t="s">
         <v>59</v>
       </c>
-      <c r="C10" s="3"/>
-      <c r="E10">
+      <c r="C10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="F10">
         <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1375,7 +1402,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1400,10 +1427,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" t="s">
         <v>71</v>
-      </c>
-      <c r="B2" t="s">
-        <v>72</v>
       </c>
       <c r="C2" t="s">
         <v>24</v>
@@ -1422,7 +1449,7 @@
   <dimension ref="B1:H4"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1448,7 +1475,7 @@
         <v>36</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>37</v>
@@ -1456,26 +1483,26 @@
     </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C4">
         <v>4</v>
@@ -1484,16 +1511,16 @@
         <v>61</v>
       </c>
       <c r="E4" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>77</v>
-      </c>
       <c r="G4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1505,8 +1532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EDEAB2A-00B2-4895-9454-5061B0D2F756}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1537,7 +1564,7 @@
         <v>44</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>45</v>
@@ -1557,13 +1584,13 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" t="s">
         <v>81</v>
       </c>
-      <c r="C2" t="s">
-        <v>82</v>
-      </c>
       <c r="G2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J2" t="s">
         <v>64</v>

</xml_diff>

<commit_message>
Update reusable actions to services
</commit_message>
<xml_diff>
--- a/customflows/src/main/resources/TestData/CustomFlowSettings.xlsx
+++ b/customflows/src/main/resources/TestData/CustomFlowSettings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Automation\Automation_Project\customflows\src\main\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6FFC341-09B5-40EC-B46B-96343E1636BF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4570EDF3-4AD1-4822-A9AD-9ED101737BDF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="908" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="908" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CFForm" sheetId="5" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="119">
   <si>
     <t>Description</t>
   </si>
@@ -144,9 +144,6 @@
     <t>Assignee</t>
   </si>
   <si>
-    <t xml:space="preserve">No Of Days </t>
-  </si>
-  <si>
     <t>Select Day</t>
   </si>
   <si>
@@ -171,9 +168,6 @@
     <t>Trigger Event</t>
   </si>
   <si>
-    <t>Restric Condition</t>
-  </si>
-  <si>
     <t>Applicable To</t>
   </si>
   <si>
@@ -183,12 +177,6 @@
     <t>Trigger Type</t>
   </si>
   <si>
-    <t>INITIATOR</t>
-  </si>
-  <si>
-    <t>Application Form</t>
-  </si>
-  <si>
     <t>Approval Flow</t>
   </si>
   <si>
@@ -243,15 +231,6 @@
     <t>Initiator</t>
   </si>
   <si>
-    <t>form:</t>
-  </si>
-  <si>
-    <t>CF Work flow Name</t>
-  </si>
-  <si>
-    <t>this is created using automation</t>
-  </si>
-  <si>
     <t>stage 1</t>
   </si>
   <si>
@@ -267,21 +246,6 @@
     <t>0</t>
   </si>
   <si>
-    <t>When</t>
-  </si>
-  <si>
-    <t>before</t>
-  </si>
-  <si>
-    <t>after</t>
-  </si>
-  <si>
-    <t>CF- Raise Requistion</t>
-  </si>
-  <si>
-    <t>created for raise requistion through automaiton</t>
-  </si>
-  <si>
     <t>Event Type</t>
   </si>
   <si>
@@ -340,6 +304,93 @@
   </si>
   <si>
     <t>Subject</t>
+  </si>
+  <si>
+    <t>Before</t>
+  </si>
+  <si>
+    <t>After</t>
+  </si>
+  <si>
+    <t>Effective Date</t>
+  </si>
+  <si>
+    <t>Select When</t>
+  </si>
+  <si>
+    <t>Approval Date</t>
+  </si>
+  <si>
+    <t>Trigger Date</t>
+  </si>
+  <si>
+    <t>CF Work flow by auto1</t>
+  </si>
+  <si>
+    <t>this is created using automation 1</t>
+  </si>
+  <si>
+    <t>No Of Days</t>
+  </si>
+  <si>
+    <t>CF Work flow by auto 0</t>
+  </si>
+  <si>
+    <t>CF Work flow by auto2</t>
+  </si>
+  <si>
+    <t>Business Flow</t>
+  </si>
+  <si>
+    <t>No Event</t>
+  </si>
+  <si>
+    <t>1,3,4</t>
+  </si>
+  <si>
+    <t>Manual</t>
+  </si>
+  <si>
+    <t>Exception</t>
+  </si>
+  <si>
+    <t>AND</t>
+  </si>
+  <si>
+    <t>1,3</t>
+  </si>
+  <si>
+    <t>Restrict Condition</t>
+  </si>
+  <si>
+    <t>ALL</t>
+  </si>
+  <si>
+    <t>Approval FLow1_2.0</t>
+  </si>
+  <si>
+    <t>Raise Requisition</t>
+  </si>
+  <si>
+    <t>CF- Raise Requisition1</t>
+  </si>
+  <si>
+    <t>CF- Raise Requisition2</t>
+  </si>
+  <si>
+    <t>created for raise requisition through automaiton1</t>
+  </si>
+  <si>
+    <t>created for raise requisition through automaiton2</t>
+  </si>
+  <si>
+    <t>IsParent</t>
+  </si>
+  <si>
+    <t>ALL,TYP</t>
+  </si>
+  <si>
+    <t>TYP,BAND</t>
   </si>
 </sst>
 </file>
@@ -676,7 +727,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -698,44 +749,44 @@
         <v>21</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" t="s">
         <v>39</v>
       </c>
-      <c r="B2" t="s">
-        <v>40</v>
-      </c>
       <c r="C2" s="4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D2" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="E2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D3" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="E3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -746,49 +797,69 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D08932F6-461B-42CB-A967-18AA58992A25}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M17" activeCellId="1" sqref="B4 M17"/>
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
+      <c r="F1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -820,7 +891,7 @@
         <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>19</v>
@@ -831,10 +902,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D2" t="s">
         <v>24</v>
@@ -845,10 +916,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D3" t="s">
         <v>25</v>
@@ -859,13 +930,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B4" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D4" t="s">
         <v>25</v>
@@ -876,13 +947,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="B5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" t="s">
         <v>56</v>
-      </c>
-      <c r="C5" t="s">
-        <v>60</v>
       </c>
       <c r="D5" t="s">
         <v>25</v>
@@ -893,10 +964,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D6" t="s">
         <v>25</v>
@@ -907,13 +978,13 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" t="s">
         <v>58</v>
-      </c>
-      <c r="C7" t="s">
-        <v>62</v>
       </c>
       <c r="D7" t="s">
         <v>24</v>
@@ -924,10 +995,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B8" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" t="s">
@@ -980,7 +1051,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>
@@ -994,7 +1065,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
@@ -1043,7 +1114,7 @@
         <v>15</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>26</v>
@@ -1072,10 +1143,10 @@
         <v>25</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="H2" t="s">
         <v>25</v>
@@ -1089,7 +1160,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="C3" t="s">
         <v>25</v>
@@ -1101,7 +1172,7 @@
         <v>25</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="H3" t="s">
         <v>25</v>
@@ -1121,7 +1192,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1140,18 +1211,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="B3" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1164,8 +1235,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64379857-4A16-4890-9E2A-322439F6ECD4}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1188,16 +1259,16 @@
         <v>29</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>30</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>31</v>
@@ -1208,16 +1279,16 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>10</v>
@@ -1228,16 +1299,16 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="B3" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="E3" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>10</v>
@@ -1248,22 +1319,22 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="B4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D4" t="s">
         <v>56</v>
       </c>
-      <c r="C4" t="s">
-        <v>96</v>
-      </c>
-      <c r="D4" t="s">
-        <v>60</v>
-      </c>
       <c r="E4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>10</v>
@@ -1277,13 +1348,13 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F5">
         <v>2</v>
@@ -1297,19 +1368,19 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="B6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>10</v>
@@ -1320,19 +1391,19 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="B7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" t="s">
+        <v>84</v>
+      </c>
+      <c r="D7" t="s">
         <v>56</v>
       </c>
-      <c r="C7" t="s">
-        <v>96</v>
-      </c>
-      <c r="D7" t="s">
-        <v>60</v>
-      </c>
       <c r="F7" s="8" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
@@ -1342,10 +1413,10 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C8" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F8">
         <v>2</v>
@@ -1356,13 +1427,13 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" t="s">
         <v>58</v>
-      </c>
-      <c r="C9" t="s">
-        <v>58</v>
-      </c>
-      <c r="D9" t="s">
-        <v>62</v>
       </c>
       <c r="F9">
         <v>3</v>
@@ -1373,10 +1444,10 @@
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C10" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D10" s="3"/>
       <c r="F10">
@@ -1385,10 +1456,10 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C11" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1399,15 +1470,16 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E12E28B-629D-4930-B6C7-4391C2FFD38B}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1427,16 +1499,44 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>99</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>97</v>
       </c>
       <c r="C2" t="s">
         <v>24</v>
       </c>
-      <c r="D2" t="s">
-        <v>62</v>
+      <c r="D2" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1446,81 +1546,283 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{694225E5-F037-4447-AFD5-F64457ED6843}">
-  <dimension ref="B1:H4"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>29</v>
+        <v>88</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>35</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>66</v>
+      </c>
       <c r="B3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="G3" t="s">
+        <v>90</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G4" t="s">
+        <v>91</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="G3" t="s">
-        <v>78</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C4">
-        <v>4</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="G5" t="s">
+        <v>90</v>
+      </c>
+      <c r="H5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="G6" t="s">
+        <v>91</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" t="s">
+        <v>84</v>
+      </c>
+      <c r="D7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="G4" t="s">
-        <v>79</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>75</v>
+      <c r="G7" t="s">
+        <v>90</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G8" t="s">
+        <v>91</v>
+      </c>
+      <c r="H8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="G9" t="s">
+        <v>90</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G10" t="s">
+        <v>91</v>
+      </c>
+      <c r="H10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G11" t="s">
+        <v>90</v>
+      </c>
+      <c r="H11" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1530,70 +1832,122 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EDEAB2A-00B2-4895-9454-5061B0D2F756}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>3</v>
+      <c r="K1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>111</v>
       </c>
       <c r="B2" t="s">
-        <v>80</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>81</v>
+        <v>112</v>
+      </c>
+      <c r="D2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F2" t="s">
+        <v>101</v>
       </c>
       <c r="G2" t="s">
-        <v>83</v>
-      </c>
-      <c r="J2" t="s">
-        <v>64</v>
+        <v>102</v>
+      </c>
+      <c r="H2" t="s">
+        <v>71</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D3" t="s">
+        <v>115</v>
+      </c>
+      <c r="F3" t="s">
+        <v>101</v>
+      </c>
+      <c r="G3" t="s">
+        <v>102</v>
+      </c>
+      <c r="H3" t="s">
+        <v>106</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>